<commit_message>
Added TestRunner to execute the test scripts automatically.
</commit_message>
<xml_diff>
--- a/MoE.ERS.Tests.Automation.DataSource/TestData.xlsx
+++ b/MoE.ERS.Tests.Automation.DataSource/TestData.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
-    <sheet name="ApplicationConfiguration" sheetId="9" r:id="rId1"/>
+    <sheet name="LogInConfiguration" sheetId="9" r:id="rId1"/>
     <sheet name="ReportConfiguration" sheetId="11" r:id="rId2"/>
     <sheet name="Welcome" sheetId="10" r:id="rId3"/>
     <sheet name="FindFormRT" sheetId="12" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Welcome!$B$1:$B$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Welcome!$D$1:$D$9</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
   <si>
     <t>UserName</t>
   </si>
@@ -84,9 +84,6 @@
     <t>TestReport</t>
   </si>
   <si>
-    <t>D:\Ayyappan\Official\ERS\LocalRepository\MoE.ERS.Tests.Automation\MoE.ERS.Tests.Automation.TestRunner\</t>
-  </si>
-  <si>
     <t>ScreenShotPath</t>
   </si>
   <si>
@@ -238,6 +235,27 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>CanExecute</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TestContainerName</t>
+  </si>
+  <si>
+    <t>FindAFormRTTestScripts</t>
+  </si>
+  <si>
+    <t>WelcomeTestScripts</t>
+  </si>
+  <si>
+    <t>D:\Ayyappan\Official\ERS\</t>
   </si>
 </sst>
 </file>
@@ -580,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -636,7 +654,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -657,7 +675,7 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -668,10 +686,10 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -681,44 +699,61 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B9"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -726,326 +761,490 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
         <v>66</v>
       </c>
-      <c r="J1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+      <c r="K16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>72</v>
+      </c>
+      <c r="K18" t="s">
         <v>41</v>
       </c>
-      <c r="M1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" t="s">
-        <v>37</v>
-      </c>
-      <c r="O7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" t="s">
-        <v>52</v>
-      </c>
-      <c r="O8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s">
         <v>42</v>
       </c>
-      <c r="O9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10">
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25" t="s">
+        <v>41</v>
+      </c>
+      <c r="L25">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="I17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17" t="s">
-        <v>40</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="O17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>68</v>
-      </c>
-      <c r="I18" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="K18" t="s">
-        <v>40</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="M25" t="s">
         <v>69</v>
-      </c>
-      <c r="I25" t="s">
-        <v>42</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="K25" t="s">
-        <v>70</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25" t="s">
-        <v>44</v>
       </c>
       <c r="N25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O25" t="s">
+        <v>43</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>47</v>
-      </c>
-      <c r="N27">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="P27">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the TestRunner changes.
</commit_message>
<xml_diff>
--- a/MoE.ERS.Tests.Automation.DataSource/TestData.xlsx
+++ b/MoE.ERS.Tests.Automation.DataSource/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LogInConfiguration" sheetId="9" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="FindFormRT" sheetId="12" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Welcome!$D$1:$D$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Welcome!$D$1:$D$7</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="83">
   <si>
     <t>UserName</t>
   </si>
@@ -243,9 +243,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>TestContainerName</t>
   </si>
   <si>
@@ -255,7 +252,28 @@
     <t>WelcomeTestScripts</t>
   </si>
   <si>
-    <t>D:\Ayyappan\Official\ERS\</t>
+    <t>n</t>
+  </si>
+  <si>
+    <t>D:\Ayyappan\Official\ERS\Latest-Nunit\MoE.ERS.Tests.Automation\MoE.ERS.Tests.Automation.TestRunner\Reports\</t>
+  </si>
+  <si>
+    <t>D:\Ayyappan\Official\ERS\Latest-Nunit\MoE.ERS.Tests.Automation\MoE.ERS.Tests.Automation.TestRunner\Screenshots\</t>
+  </si>
+  <si>
+    <t>ValidateMakeANewRequestButtonExistence</t>
+  </si>
+  <si>
+    <t>ValidateMakeANewRequestButtonEnabled</t>
+  </si>
+  <si>
+    <t>ValidateViewAllRequestsButtonEnabled</t>
+  </si>
+  <si>
+    <t>ValidateRequestButtonsAlignment</t>
+  </si>
+  <si>
+    <t>MakeANewRequest</t>
   </si>
 </sst>
 </file>
@@ -598,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -653,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -689,7 +707,7 @@
         <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -699,9 +717,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -713,7 +733,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -727,13 +747,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -741,16 +761,82 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -764,8 +850,8 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -791,7 +877,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -844,35 +930,35 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>
@@ -880,13 +966,13 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
         <v>64</v>
@@ -894,24 +980,24 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K7" t="s">
         <v>36</v>
@@ -922,13 +1008,13 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K8" t="s">
         <v>51</v>
@@ -939,13 +1025,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K9" t="s">
         <v>41</v>
@@ -956,13 +1042,13 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
         <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K10" t="s">
         <v>41</v>
@@ -973,24 +1059,27 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
         <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>53</v>
@@ -1004,13 +1093,13 @@
     </row>
     <row r="13" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
         <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K13" t="s">
         <v>41</v>
@@ -1021,13 +1110,13 @@
     </row>
     <row r="14" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K14" t="s">
         <v>41</v>
@@ -1038,13 +1127,13 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G15" t="s">
         <v>56</v>
@@ -1058,13 +1147,13 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
         <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K16" t="s">
         <v>41</v>
@@ -1075,13 +1164,13 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K17" t="s">
         <v>41</v>
@@ -1101,13 +1190,13 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
         <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K18" t="s">
         <v>41</v>
@@ -1124,13 +1213,13 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
         <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H19" t="s">
         <v>58</v>
@@ -1138,35 +1227,35 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
         <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
         <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I22" t="s">
         <v>61</v>
@@ -1174,35 +1263,35 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
         <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
         <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K25" t="s">
         <v>41</v>
@@ -1225,24 +1314,24 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
         <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
         <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="P27">
         <v>1</v>

</xml_diff>

<commit_message>
Chek in the changes done Create method in DriverFactory class.
</commit_message>
<xml_diff>
--- a/MoE.ERS.Tests.Automation.DataSource/TestData.xlsx
+++ b/MoE.ERS.Tests.Automation.DataSource/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LogInConfiguration" sheetId="9" r:id="rId1"/>
@@ -617,7 +617,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -849,9 +849,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1065,7 +1065,7 @@
         <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -1076,7 +1076,7 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
@@ -1099,7 +1099,7 @@
         <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K13" t="s">
         <v>41</v>
@@ -1116,7 +1116,7 @@
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K14" t="s">
         <v>41</v>
@@ -1133,7 +1133,7 @@
         <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G15" t="s">
         <v>56</v>
@@ -1153,7 +1153,7 @@
         <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K16" t="s">
         <v>41</v>
@@ -1196,7 +1196,7 @@
         <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K18" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Committed the changes done
</commit_message>
<xml_diff>
--- a/MoE.ERS.Tests.Automation.DataSource/TestData.xlsx
+++ b/MoE.ERS.Tests.Automation.DataSource/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LogInConfiguration" sheetId="9" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="86">
   <si>
     <t>UserName</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>MakeANewRequest</t>
+  </si>
+  <si>
+    <t>Er</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Aded</t>
   </si>
 </sst>
 </file>
@@ -617,7 +626,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -719,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -767,7 +776,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -781,7 +790,7 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -792,7 +801,7 @@
         <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -803,7 +812,7 @@
         <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -814,7 +823,7 @@
         <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -825,7 +834,7 @@
         <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -836,7 +845,7 @@
         <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -847,11 +856,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1065,7 +1074,7 @@
         <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -1076,7 +1085,7 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
@@ -1099,10 +1108,10 @@
         <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="K13" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -1116,10 +1125,10 @@
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="K14" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -1133,13 +1142,13 @@
         <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G15" t="s">
         <v>56</v>
       </c>
       <c r="K15" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1153,7 +1162,7 @@
         <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="K16" t="s">
         <v>41</v>
@@ -1193,10 +1202,10 @@
         <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="K18" t="s">
         <v>41</v>
@@ -1205,24 +1214,36 @@
         <v>1</v>
       </c>
       <c r="M18" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
+      <c r="Q18" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
         <v>75</v>
       </c>
-      <c r="H19" t="s">
-        <v>58</v>
+      <c r="K19" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
@@ -1230,10 +1251,13 @@
         <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>75</v>
+      </c>
+      <c r="H20" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
@@ -1241,7 +1265,7 @@
         <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
         <v>75</v>
@@ -1252,13 +1276,10 @@
         <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
         <v>75</v>
-      </c>
-      <c r="I22" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
@@ -1266,10 +1287,13 @@
         <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
         <v>75</v>
+      </c>
+      <c r="I23" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
@@ -1277,7 +1301,7 @@
         <v>73</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
         <v>75</v>
@@ -1288,28 +1312,10 @@
         <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
         <v>75</v>
-      </c>
-      <c r="K25" t="s">
-        <v>41</v>
-      </c>
-      <c r="L25">
-        <v>1</v>
-      </c>
-      <c r="M25" t="s">
-        <v>69</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25" t="s">
-        <v>43</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
@@ -1317,10 +1323,28 @@
         <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
         <v>75</v>
+      </c>
+      <c r="K26" t="s">
+        <v>41</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26" t="s">
+        <v>69</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
@@ -1328,12 +1352,23 @@
         <v>73</v>
       </c>
       <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
         <v>46</v>
       </c>
-      <c r="C27" t="s">
-        <v>75</v>
-      </c>
-      <c r="P27">
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="P28">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Committed the changes ElementIdentifiers.
</commit_message>
<xml_diff>
--- a/MoE.ERS.Tests.Automation.DataSource/TestData.xlsx
+++ b/MoE.ERS.Tests.Automation.DataSource/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LogInConfiguration" sheetId="9" r:id="rId1"/>
@@ -681,7 +681,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -762,7 +762,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -858,9 +858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1040,10 +1040,13 @@
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
-      </c>
-      <c r="K9" t="s">
-        <v>41</v>
+        <v>71</v>
+      </c>
+      <c r="K9">
+        <v>36863</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
       </c>
       <c r="Q9" t="s">
         <v>50</v>
@@ -1305,6 +1308,15 @@
       </c>
       <c r="C24" t="s">
         <v>75</v>
+      </c>
+      <c r="K24" t="s">
+        <v>41</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">

</xml_diff>